<commit_message>
Correct adult target & upload all colab results
</commit_message>
<xml_diff>
--- a/results_colab/results_no_search.xlsx
+++ b/results_colab/results_no_search.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,16 +462,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>0.990159901599016</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.998769987699877</v>
       </c>
-      <c r="B2" t="n">
-        <v>0.995079950799508</v>
-      </c>
       <c r="C2" t="n">
-        <v>0.995079950799508</v>
+        <v>0.993849938499385</v>
       </c>
       <c r="D2" t="n">
-        <v>0.997539975399754</v>
+        <v>0.996309963099631</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -481,16 +481,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>0.990159901599016</v>
       </c>
       <c r="B3" t="n">
-        <v>0.998769987699877</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.995079950799508</v>
+        <v>0.985239852398524</v>
       </c>
       <c r="D3" t="n">
-        <v>0.992619926199262</v>
+        <v>0.982779827798278</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -509,7 +509,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.998769987699877</v>
+        <v>0.988929889298893</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -519,16 +519,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.997539975399754</v>
+        <v>0.995079950799508</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0.993849938499385</v>
+        <v>0.9864698646986469</v>
       </c>
       <c r="D5" t="n">
-        <v>0.993849938499385</v>
+        <v>0.9876998769987699</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -544,10 +544,10 @@
         <v>0.9987684729064039</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9987684729064039</v>
+        <v>0.9926108374384236</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9926108374384236</v>
+        <v>0.9876847290640394</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -557,16 +557,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.9975369458128078</v>
+        <v>0.9963054187192119</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9975369458128078</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9938423645320197</v>
+        <v>0.9950738916256158</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9963054187192119</v>
+        <v>0.9815270935960592</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -576,16 +576,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1</v>
+        <v>0.9913793103448276</v>
       </c>
       <c r="B8" t="n">
         <v>0.9987684729064039</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9987684729064039</v>
+        <v>0.9938423645320197</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9950738916256158</v>
+        <v>0.9901477832512315</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -595,16 +595,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1</v>
+        <v>0.9667487684729064</v>
       </c>
       <c r="B9" t="n">
-        <v>0.9987684729064039</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
         <v>0.9926108374384236</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9987684729064039</v>
+        <v>0.9802955665024631</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -617,13 +617,13 @@
         <v>0.9938423645320197</v>
       </c>
       <c r="B10" t="n">
-        <v>0.9975369458128078</v>
+        <v>0.9963054187192119</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9963054187192119</v>
+        <v>0.9938423645320197</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9901477832512315</v>
+        <v>0.9827586206896551</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -633,16 +633,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>0.9938423645320197</v>
+      </c>
+      <c r="B11" t="n">
         <v>0.9987684729064039</v>
       </c>
-      <c r="B11" t="n">
-        <v>0.9950738916256158</v>
-      </c>
       <c r="C11" t="n">
-        <v>0.9926108374384236</v>
+        <v>0.9938423645320197</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9950738916256158</v>
+        <v>0.9913793103448276</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -652,16 +652,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.5560344827586207</v>
+        <v>0.8580588105239885</v>
       </c>
       <c r="B12" t="n">
-        <v>0.5560344827586207</v>
+        <v>0.8589431793057705</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5646551724137931</v>
+        <v>0.8633650232146806</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5571120689655172</v>
+        <v>0.863143931019235</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -671,16 +671,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.5689655172413793</v>
+        <v>0.8651337607782446</v>
       </c>
       <c r="B13" t="n">
-        <v>0.572198275862069</v>
+        <v>0.8671235905372541</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5732758620689655</v>
+        <v>0.8686712359053725</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5592672413793104</v>
+        <v>0.8695556046871545</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -690,16 +690,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.5495689655172413</v>
+        <v>0.8615656789031402</v>
       </c>
       <c r="B14" t="n">
-        <v>0.5538793103448276</v>
+        <v>0.8637770897832817</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5549568965517241</v>
+        <v>0.8642193719593101</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5301724137931034</v>
+        <v>0.8657673595754091</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -709,16 +709,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.5614224137931034</v>
+        <v>0.8710747456877488</v>
       </c>
       <c r="B15" t="n">
-        <v>0.5678879310344828</v>
+        <v>0.8761609907120743</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5689655172413793</v>
+        <v>0.8752764263600177</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5732758620689655</v>
+        <v>0.8728438743918621</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -728,16 +728,16 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.5603448275862069</v>
+        <v>0.8586908447589562</v>
       </c>
       <c r="B16" t="n">
-        <v>0.5657327586206896</v>
+        <v>0.8622291021671826</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5646551724137931</v>
+        <v>0.865546218487395</v>
       </c>
       <c r="D16" t="n">
-        <v>0.5592672413793104</v>
+        <v>0.862671384343211</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -747,16 +747,16 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.5657327586206896</v>
+        <v>0.8538257408226448</v>
       </c>
       <c r="B17" t="n">
-        <v>0.5786637931034483</v>
+        <v>0.8646616541353384</v>
       </c>
       <c r="C17" t="n">
-        <v>0.5829741379310345</v>
+        <v>0.862671384343211</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5517241379310345</v>
+        <v>0.862671384343211</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -766,16 +766,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.5625</v>
+        <v>0.8664307828394515</v>
       </c>
       <c r="B18" t="n">
-        <v>0.5732758620689655</v>
+        <v>0.8653250773993808</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5797413793103449</v>
+        <v>0.8701901813356921</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5689655172413793</v>
+        <v>0.8659885006634233</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -785,16 +785,16 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.5732758620689655</v>
+        <v>0.865546218487395</v>
       </c>
       <c r="B19" t="n">
-        <v>0.5743534482758621</v>
+        <v>0.871517027863777</v>
       </c>
       <c r="C19" t="n">
-        <v>0.5818965517241379</v>
+        <v>0.8730650154798761</v>
       </c>
       <c r="D19" t="n">
-        <v>0.5549568965517241</v>
+        <v>0.8693056169836355</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -804,16 +804,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.5571120689655172</v>
+        <v>0.8704113224237063</v>
       </c>
       <c r="B20" t="n">
-        <v>0.5743534482758621</v>
+        <v>0.8719593100398054</v>
       </c>
       <c r="C20" t="n">
-        <v>0.5765086206896551</v>
+        <v>0.8759398496240601</v>
       </c>
       <c r="D20" t="n">
-        <v>0.5668103448275862</v>
+        <v>0.8706324635117205</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -823,16 +823,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.5635775862068966</v>
+        <v>0.8675364882795223</v>
       </c>
       <c r="B21" t="n">
-        <v>0.5657327586206896</v>
+        <v>0.8681999115435648</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5678879310344828</v>
+        <v>0.8759398496240601</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5431034482758621</v>
+        <v>0.8726227333038479</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -842,16 +842,16 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.8056737588652483</v>
+        <v>0.8</v>
       </c>
       <c r="B22" t="n">
+        <v>0.8085106382978723</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.8028368794326242</v>
+      </c>
+      <c r="D22" t="n">
         <v>0.8070921985815603</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.8099290780141843</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.8014184397163121</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -861,16 +861,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.8085106382978723</v>
+        <v>0.8042553191489362</v>
       </c>
       <c r="B23" t="n">
-        <v>0.8085106382978723</v>
+        <v>0.7929078014184398</v>
       </c>
       <c r="C23" t="n">
-        <v>0.8099290780141843</v>
+        <v>0.8141843971631205</v>
       </c>
       <c r="D23" t="n">
-        <v>0.8113475177304964</v>
+        <v>0.8042553191489362</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -880,16 +880,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.7914893617021277</v>
+        <v>0.7971631205673759</v>
       </c>
       <c r="B24" t="n">
-        <v>0.7914893617021277</v>
+        <v>0.7843971631205674</v>
       </c>
       <c r="C24" t="n">
-        <v>0.7886524822695036</v>
+        <v>0.7815602836879433</v>
       </c>
       <c r="D24" t="n">
-        <v>0.8085106382978723</v>
+        <v>0.7787234042553192</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -899,16 +899,16 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.7840909090909091</v>
+        <v>0.7826704545454546</v>
       </c>
       <c r="B25" t="n">
-        <v>0.7869318181818182</v>
+        <v>0.7826704545454546</v>
       </c>
       <c r="C25" t="n">
-        <v>0.7826704545454546</v>
+        <v>0.78125</v>
       </c>
       <c r="D25" t="n">
-        <v>0.7798295454545454</v>
+        <v>0.7897727272727273</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -918,16 +918,16 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.7954545454545454</v>
+        <v>0.8068181818181818</v>
       </c>
       <c r="B26" t="n">
-        <v>0.7926136363636364</v>
+        <v>0.7741477272727273</v>
       </c>
       <c r="C26" t="n">
-        <v>0.796875</v>
+        <v>0.7911931818181818</v>
       </c>
       <c r="D26" t="n">
-        <v>0.796875</v>
+        <v>0.7940340909090909</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -937,16 +937,16 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.8053977272727273</v>
+        <v>0.8068181818181818</v>
       </c>
       <c r="B27" t="n">
-        <v>0.8039772727272727</v>
+        <v>0.7755681818181818</v>
       </c>
       <c r="C27" t="n">
-        <v>0.7982954545454546</v>
+        <v>0.7897727272727273</v>
       </c>
       <c r="D27" t="n">
-        <v>0.7769886363636364</v>
+        <v>0.7755681818181818</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -956,16 +956,16 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.7997159090909091</v>
+        <v>0.8025568181818182</v>
       </c>
       <c r="B28" t="n">
-        <v>0.8011363636363636</v>
+        <v>0.7883522727272727</v>
       </c>
       <c r="C28" t="n">
-        <v>0.8011363636363636</v>
+        <v>0.7926136363636364</v>
       </c>
       <c r="D28" t="n">
-        <v>0.796875</v>
+        <v>0.7911931818181818</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -975,16 +975,16 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.7997159090909091</v>
+        <v>0.8082386363636364</v>
       </c>
       <c r="B29" t="n">
-        <v>0.8025568181818182</v>
+        <v>0.7613636363636364</v>
       </c>
       <c r="C29" t="n">
-        <v>0.8082386363636364</v>
+        <v>0.7954545454545454</v>
       </c>
       <c r="D29" t="n">
-        <v>0.7954545454545454</v>
+        <v>0.7940340909090909</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -994,16 +994,16 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.7997159090909091</v>
+        <v>0.7954545454545454</v>
       </c>
       <c r="B30" t="n">
-        <v>0.7982954545454546</v>
+        <v>0.7769886363636364</v>
       </c>
       <c r="C30" t="n">
-        <v>0.7997159090909091</v>
+        <v>0.7755681818181818</v>
       </c>
       <c r="D30" t="n">
-        <v>0.796875</v>
+        <v>0.8039772727272727</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1013,16 +1013,16 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.7997159090909091</v>
+        <v>0.7954545454545454</v>
       </c>
       <c r="B31" t="n">
-        <v>0.796875</v>
+        <v>0.7727272727272727</v>
       </c>
       <c r="C31" t="n">
-        <v>0.7869318181818182</v>
+        <v>0.7741477272727273</v>
       </c>
       <c r="D31" t="n">
-        <v>0.7926136363636364</v>
+        <v>0.7883522727272727</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1032,16 +1032,16 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.9975000000000001</v>
+        <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>0.99875</v>
+        <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>0.99875</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>0.99875</v>
+        <v>1</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1051,16 +1051,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.99875</v>
+        <v>1</v>
       </c>
       <c r="B33" t="n">
         <v>1</v>
       </c>
       <c r="C33" t="n">
-        <v>0.99875</v>
+        <v>0.998</v>
       </c>
       <c r="D33" t="n">
-        <v>0.99875</v>
+        <v>1</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1070,16 +1070,16 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.99625</v>
+        <v>0.998</v>
       </c>
       <c r="B34" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>0.998</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>0.998</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.99875</v>
+        <v>0.999</v>
       </c>
       <c r="B35" t="n">
         <v>1</v>
@@ -1098,7 +1098,7 @@
         <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1114,7 +1114,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="n">
-        <v>1</v>
+        <v>0.989</v>
       </c>
       <c r="D36" t="n">
         <v>1</v>
@@ -1127,16 +1127,16 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.99875</v>
+        <v>1</v>
       </c>
       <c r="B37" t="n">
-        <v>0.99875</v>
+        <v>0.999</v>
       </c>
       <c r="C37" t="n">
-        <v>0.99875</v>
+        <v>0.992</v>
       </c>
       <c r="D37" t="n">
-        <v>0.99875</v>
+        <v>0.999</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1146,16 +1146,16 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.99875</v>
+        <v>1</v>
       </c>
       <c r="B38" t="n">
-        <v>0.99875</v>
+        <v>1</v>
       </c>
       <c r="C38" t="n">
-        <v>0.9975000000000001</v>
+        <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>0.9975000000000001</v>
+        <v>1</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1171,7 +1171,7 @@
         <v>1</v>
       </c>
       <c r="C39" t="n">
-        <v>0.99875</v>
+        <v>0.998</v>
       </c>
       <c r="D39" t="n">
         <v>1</v>
@@ -1184,16 +1184,16 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="B40" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="C40" t="n">
-        <v>0.99875</v>
+        <v>0.997</v>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1203,16 +1203,16 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.9975000000000001</v>
+        <v>0.999</v>
       </c>
       <c r="B41" t="n">
-        <v>0.99875</v>
+        <v>0.999</v>
       </c>
       <c r="C41" t="n">
-        <v>0.99875</v>
+        <v>0.998</v>
       </c>
       <c r="D41" t="n">
-        <v>0.99875</v>
+        <v>0.999</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1263,7 +1263,7 @@
         <v>0.9</v>
       </c>
       <c r="B44" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C44" t="n">
         <v>1</v>
@@ -1304,7 +1304,7 @@
         <v>0.9</v>
       </c>
       <c r="C46" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D46" t="n">
         <v>0.9</v>
@@ -1336,7 +1336,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="B48" t="n">
         <v>0.9</v>
@@ -1345,7 +1345,7 @@
         <v>0.9</v>
       </c>
       <c r="D48" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="B49" t="n">
         <v>1</v>
@@ -1377,13 +1377,13 @@
         <v>0.8</v>
       </c>
       <c r="B50" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="C50" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" t="n">
         <v>0.9</v>
-      </c>
-      <c r="D50" t="n">
-        <v>1</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1393,7 +1393,7 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="B51" t="n">
         <v>0.9</v>
@@ -1418,10 +1418,10 @@
         <v>0.875</v>
       </c>
       <c r="C52" t="n">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="D52" t="n">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1478,7 +1478,7 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="D55" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1602,77 +1602,77 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>0.6</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="B62" t="n">
-        <v>0.7</v>
+        <v>0.79</v>
       </c>
       <c r="C62" t="n">
-        <v>0.65</v>
+        <v>0.805</v>
       </c>
       <c r="D62" t="n">
-        <v>0.6</v>
+        <v>0.85</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>weather</t>
+          <t>IMDB reviews</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>0.7</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="B63" t="n">
-        <v>0.6</v>
+        <v>0.805</v>
       </c>
       <c r="C63" t="n">
-        <v>0.6</v>
+        <v>0.835</v>
       </c>
       <c r="D63" t="n">
-        <v>0.6</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>weather</t>
+          <t>IMDB reviews</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>0.5</v>
+        <v>0.76</v>
       </c>
       <c r="B64" t="n">
-        <v>0.55</v>
+        <v>0.77</v>
       </c>
       <c r="C64" t="n">
-        <v>0.5</v>
+        <v>0.775</v>
       </c>
       <c r="D64" t="n">
-        <v>0.5</v>
+        <v>0.76</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>weather</t>
+          <t>IMDB reviews</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>0.55</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="B65" t="n">
-        <v>0.6</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="C65" t="n">
-        <v>0.55</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="D65" t="n">
-        <v>0.7</v>
+        <v>0.82</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>weather</t>
+          <t>IMDB reviews</t>
         </is>
       </c>
     </row>
@@ -1681,93 +1681,93 @@
         <v>0.8</v>
       </c>
       <c r="B66" t="n">
-        <v>0.8</v>
+        <v>0.765</v>
       </c>
       <c r="C66" t="n">
-        <v>0.7</v>
+        <v>0.805</v>
       </c>
       <c r="D66" t="n">
-        <v>0.65</v>
+        <v>0.82</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>weather</t>
+          <t>IMDB reviews</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>0.65</v>
+        <v>0.805</v>
       </c>
       <c r="B67" t="n">
-        <v>0.7</v>
+        <v>0.825</v>
       </c>
       <c r="C67" t="n">
-        <v>0.65</v>
+        <v>0.805</v>
       </c>
       <c r="D67" t="n">
-        <v>0.6</v>
+        <v>0.825</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>weather</t>
+          <t>IMDB reviews</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>0.6</v>
+        <v>0.795</v>
       </c>
       <c r="B68" t="n">
-        <v>0.55</v>
+        <v>0.775</v>
       </c>
       <c r="C68" t="n">
-        <v>0.5</v>
+        <v>0.795</v>
       </c>
       <c r="D68" t="n">
-        <v>0.55</v>
+        <v>0.785</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>weather</t>
+          <t>IMDB reviews</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>0.55</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="B69" t="n">
-        <v>0.65</v>
+        <v>0.835</v>
       </c>
       <c r="C69" t="n">
-        <v>0.6</v>
+        <v>0.785</v>
       </c>
       <c r="D69" t="n">
-        <v>0.75</v>
+        <v>0.83</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>weather</t>
+          <t>IMDB reviews</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>0.55</v>
+        <v>0.83</v>
       </c>
       <c r="B70" t="n">
-        <v>0.5</v>
+        <v>0.84</v>
       </c>
       <c r="C70" t="n">
-        <v>0.55</v>
+        <v>0.85</v>
       </c>
       <c r="D70" t="n">
-        <v>0.65</v>
+        <v>0.875</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>weather</t>
+          <t>IMDB reviews</t>
         </is>
       </c>
     </row>
@@ -1776,205 +1776,15 @@
         <v>0.8</v>
       </c>
       <c r="B71" t="n">
-        <v>0.8</v>
+        <v>0.765</v>
       </c>
       <c r="C71" t="n">
-        <v>0.85</v>
+        <v>0.79</v>
       </c>
       <c r="D71" t="n">
-        <v>0.75</v>
+        <v>0.805</v>
       </c>
       <c r="E71" t="inlineStr">
-        <is>
-          <t>weather</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>0.755</v>
-      </c>
-      <c r="B72" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="C72" t="n">
-        <v>0.745</v>
-      </c>
-      <c r="D72" t="n">
-        <v>0.735</v>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>IMDB reviews</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="B73" t="n">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="C73" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="D73" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>IMDB reviews</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="B74" t="n">
-        <v>0.775</v>
-      </c>
-      <c r="C74" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="D74" t="n">
-        <v>0.765</v>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>IMDB reviews</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>0.765</v>
-      </c>
-      <c r="B75" t="n">
-        <v>0.745</v>
-      </c>
-      <c r="C75" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="D75" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>IMDB reviews</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>0.775</v>
-      </c>
-      <c r="B76" t="n">
-        <v>0.795</v>
-      </c>
-      <c r="C76" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="D76" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>IMDB reviews</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>0.775</v>
-      </c>
-      <c r="B77" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="C77" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="D77" t="n">
-        <v>0.755</v>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>IMDB reviews</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="B78" t="n">
-        <v>0.855</v>
-      </c>
-      <c r="C78" t="n">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="D78" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>IMDB reviews</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="B79" t="n">
-        <v>0.725</v>
-      </c>
-      <c r="C79" t="n">
-        <v>0.715</v>
-      </c>
-      <c r="D79" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>IMDB reviews</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>0.775</v>
-      </c>
-      <c r="B80" t="n">
-        <v>0.76</v>
-      </c>
-      <c r="C80" t="n">
-        <v>0.795</v>
-      </c>
-      <c r="D80" t="n">
-        <v>0.775</v>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>IMDB reviews</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>0.785</v>
-      </c>
-      <c r="B81" t="n">
-        <v>0.825</v>
-      </c>
-      <c r="C81" t="n">
-        <v>0.8149999999999999</v>
-      </c>
-      <c r="D81" t="n">
-        <v>0.8149999999999999</v>
-      </c>
-      <c r="E81" t="inlineStr">
         <is>
           <t>IMDB reviews</t>
         </is>

</xml_diff>